<commit_message>
Add some notes on working with the CV script that I wrote to calculate MSE for model selection
</commit_message>
<xml_diff>
--- a/admin/model_testing_assignment.xlsx
+++ b/admin/model_testing_assignment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>users</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Cross-validated Mean-Squared Error</t>
   </si>
   <si>
+    <t>If you want to use CV code I wrote you can follow:</t>
+  </si>
+  <si>
     <t>heavy</t>
   </si>
   <si>
@@ -35,28 +38,122 @@
     <t>jim</t>
   </si>
   <si>
+    <t>Copy and paste 06_cross_val_model_selection.R into your named folder</t>
+  </si>
+  <si>
     <t>level-log</t>
   </si>
   <si>
     <t>julian</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Ensure you have the data (named as </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">InstantCoffee.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) inside the data folder of the project directory</t>
+    </r>
+  </si>
+  <si>
     <t>log-log</t>
   </si>
   <si>
     <t>maria</t>
   </si>
   <si>
+    <t>Open the R studio project in the root directory of the project folder (this sets your working directory)</t>
+  </si>
+  <si>
     <t>light</t>
   </si>
   <si>
     <t>tina</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Run line 3 in the file (</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">source(“./r/analysis.R”)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">), this should create 3 objects, </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">coffee_clean; heavy; light</t>
+    </r>
+  </si>
+  <si>
     <t>joe</t>
   </si>
   <si>
+    <t>Change line 7 to be the users you want to model (i.e. either heavy or light)</t>
+  </si>
+  <si>
     <t>jessica</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At line 50, change the functional form of the model to be that you're working on: ie log-transform with </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">log()</t>
+    </r>
+  </si>
+  <si>
+    <t>Run the script from Step 1 onwards, it should compute a single average MSE that we can use to assess model quality.</t>
+  </si>
+  <si>
+    <t>Any questions let me know, I'll be online most/all of the day</t>
   </si>
 </sst>
 </file>
@@ -66,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -88,6 +185,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,9 +237,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -154,22 +263,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.5708502024292"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6842105263158"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="90.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -179,74 +291,126 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>174.7772</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="0" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>13</v>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change label of level-log to semi-log
</commit_message>
<xml_diff>
--- a/admin/model_testing_assignment.xlsx
+++ b/admin/model_testing_assignment.xlsx
@@ -41,7 +41,7 @@
     <t>Copy and paste 06_cross_val_model_selection.R into your named folder</t>
   </si>
   <si>
-    <t>level-log</t>
+    <t>Semi-log</t>
   </si>
   <si>
     <t>julian</t>
@@ -266,7 +266,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>